<commit_message>
Add the Dots Logic
</commit_message>
<xml_diff>
--- a/data/testData1.xlsx
+++ b/data/testData1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wdtablesys1-my.sharepoint.com/personal/prasad_kamble_wdtablesystems_com/Documents/Documents/PlayWrightProject/PlayWrightPOC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="11_F25DC773A252ABDACC1048D4E99B63705BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27C98C6A-D10F-4ABC-BDAB-CAF77351252A}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="11_F25DC773A252ABDACC1048D4E99B63705BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9619E1DE-054E-4DCB-B31D-58EDF6D2F7B7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testData" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="81">
   <si>
     <t>All-chips</t>
   </si>
@@ -149,6 +149,126 @@
   </si>
   <si>
     <t>3s</t>
+  </si>
+  <si>
+    <t>e0054001804f8e50</t>
+  </si>
+  <si>
+    <t>e0054001804f93d4</t>
+  </si>
+  <si>
+    <t>e0054001804fa1d4</t>
+  </si>
+  <si>
+    <t>e0054001f00e112a</t>
+  </si>
+  <si>
+    <t>e0054001f00e1c3c</t>
+  </si>
+  <si>
+    <t>e0054001121a1753</t>
+  </si>
+  <si>
+    <t>e0054001121a1754</t>
+  </si>
+  <si>
+    <t>e0054001121a17dd</t>
+  </si>
+  <si>
+    <t>e0054001121a17ec</t>
+  </si>
+  <si>
+    <t>e00540011226ac40</t>
+  </si>
+  <si>
+    <t>e04ff0010014acac</t>
+  </si>
+  <si>
+    <t>e04ff0010014acce</t>
+  </si>
+  <si>
+    <t>e04ff0010014ace2</t>
+  </si>
+  <si>
+    <t>e04ff0010014acf2</t>
+  </si>
+  <si>
+    <t>e04ff0010014ad0f</t>
+  </si>
+  <si>
+    <t>e04ff0010014ad26</t>
+  </si>
+  <si>
+    <t>e04ff0010014ad49</t>
+  </si>
+  <si>
+    <t>e04ff0010014ad5a</t>
+  </si>
+  <si>
+    <t>e04ff0010014cf66</t>
+  </si>
+  <si>
+    <t>e04ff0010014cfc5</t>
+  </si>
+  <si>
+    <t>e0054001804f7b26</t>
+  </si>
+  <si>
+    <t>e0054001804f8385</t>
+  </si>
+  <si>
+    <t>e0054001804fa787</t>
+  </si>
+  <si>
+    <t>e0054001804fb066</t>
+  </si>
+  <si>
+    <t>e0054001804fb98f</t>
+  </si>
+  <si>
+    <t>e0054001121a17f4</t>
+  </si>
+  <si>
+    <t>e0054001121a1803</t>
+  </si>
+  <si>
+    <t>e0054001121a180d</t>
+  </si>
+  <si>
+    <t>e0054001121a1833</t>
+  </si>
+  <si>
+    <t>e0054001121a1844</t>
+  </si>
+  <si>
+    <t>e0054001121a180e</t>
+  </si>
+  <si>
+    <t>e0054001121a1819</t>
+  </si>
+  <si>
+    <t>e0054001121a1822</t>
+  </si>
+  <si>
+    <t>e0054001121a183e</t>
+  </si>
+  <si>
+    <t>e0054001121a1840</t>
+  </si>
+  <si>
+    <t>e00540011212acfe</t>
+  </si>
+  <si>
+    <t>e0054001120dc6b3</t>
+  </si>
+  <si>
+    <t>e00540011212ac3e</t>
+  </si>
+  <si>
+    <t>e0054001120db6ee</t>
+  </si>
+  <si>
+    <t>e005400112138f8c</t>
   </si>
 </sst>
 </file>
@@ -492,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,10 +695,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9965AA6-5EAD-4E12-9BEA-FDC5BCC4DB29}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +929,428 @@
         <v>4</v>
       </c>
     </row>
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="3">
+        <v>500</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="3">
+        <v>500</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="3">
+        <v>500</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="3">
+        <v>500</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="3">
+        <v>500</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="3">
+        <v>500</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="3">
+        <v>500</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="3">
+        <v>500</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="3">
+        <v>500</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="3">
+        <v>500</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="3">
+        <v>500</v>
+      </c>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="3">
+        <v>500</v>
+      </c>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="3">
+        <v>500</v>
+      </c>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="3">
+        <v>500</v>
+      </c>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="3">
+        <v>500</v>
+      </c>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="3">
+        <v>500</v>
+      </c>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="3">
+        <v>500</v>
+      </c>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="3">
+        <v>500</v>
+      </c>
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="3">
+        <v>500</v>
+      </c>
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="3">
+        <v>500</v>
+      </c>
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B52" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B55" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B58" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B59" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B60" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Allure and base test add
</commit_message>
<xml_diff>
--- a/data/testData1.xlsx
+++ b/data/testData1.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="61" documentId="11_F25DC773A252ABDACC1048D4E99B63705BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9619E1DE-054E-4DCB-B31D-58EDF6D2F7B7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testData" sheetId="1" r:id="rId1"/>
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9965AA6-5EAD-4E12-9BEA-FDC5BCC4DB29}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>